<commit_message>
Mar 26 1. expanding grid 2. higher upper boudn of w 3. calculate consumption CE 4. fix the problem of constraint - (1 + R) 5. improve the plot settings 6. new results
</commit_message>
<xml_diff>
--- a/data/Conditional Survival Prob Feb 16.xlsx
+++ b/data/Conditional Survival Prob Feb 16.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>AGE</t>
   </si>
   <si>
     <t>CSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -347,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -367,6 +370,9 @@
       <c r="A2">
         <v>20</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -608,7 +614,7 @@
         <v>0.99767358158895425</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>51</v>
       </c>
@@ -616,7 +622,7 @@
         <v>0.99756358978380777</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>52</v>
       </c>
@@ -624,7 +630,7 @@
         <v>0.99742138364779875</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>53</v>
       </c>
@@ -632,7 +638,7 @@
         <v>0.99724656872017992</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>54</v>
       </c>
@@ -640,7 +646,7 @@
         <v>0.99702294701899519</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>55</v>
       </c>
@@ -648,7 +654,7 @@
         <v>0.99676038473734274</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>56</v>
       </c>
@@ -656,7 +662,7 @@
         <v>0.99645824386157456</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>57</v>
       </c>
@@ -664,7 +670,7 @@
         <v>0.9961157609649941</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>58</v>
       </c>
@@ -672,7 +678,7 @@
         <v>0.99575875091475308</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>59</v>
       </c>
@@ -680,7 +686,7 @@
         <v>0.99538124818951368</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -688,7 +694,7 @@
         <v>0.99499334421971086</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>61</v>
       </c>
@@ -696,7 +702,7 @@
         <v>0.99455650402981199</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>62</v>
       </c>
@@ -704,7 +710,7 @@
         <v>0.99405287063359804</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>63</v>
       </c>
@@ -712,7 +718,7 @@
         <v>0.99345298751958622</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>64</v>
       </c>
@@ -720,15 +726,18 @@
         <v>0.99272600934203192</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>65</v>
       </c>
       <c r="B47">
         <v>0.99188942959358262</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>66</v>
       </c>
@@ -1010,5 +1019,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Apr 4 1. negative income found 2. run all the iterations
</commit_message>
<xml_diff>
--- a/data/Conditional Survival Prob Feb 16.xlsx
+++ b/data/Conditional Survival Prob Feb 16.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>AGE</t>
   </si>
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +614,7 @@
         <v>0.99767358158895425</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>51</v>
       </c>
@@ -622,7 +622,7 @@
         <v>0.99756358978380777</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>52</v>
       </c>
@@ -630,7 +630,7 @@
         <v>0.99742138364779875</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>53</v>
       </c>
@@ -638,7 +638,7 @@
         <v>0.99724656872017992</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>54</v>
       </c>
@@ -646,7 +646,7 @@
         <v>0.99702294701899519</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>55</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0.99676038473734274</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>56</v>
       </c>
@@ -662,7 +662,7 @@
         <v>0.99645824386157456</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>57</v>
       </c>
@@ -670,7 +670,7 @@
         <v>0.9961157609649941</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>58</v>
       </c>
@@ -678,7 +678,7 @@
         <v>0.99575875091475308</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>59</v>
       </c>
@@ -686,7 +686,7 @@
         <v>0.99538124818951368</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -694,7 +694,7 @@
         <v>0.99499334421971086</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>61</v>
       </c>
@@ -702,7 +702,7 @@
         <v>0.99455650402981199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>62</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.99405287063359804</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>63</v>
       </c>
@@ -718,7 +718,7 @@
         <v>0.99345298751958622</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>64</v>
       </c>
@@ -726,18 +726,15 @@
         <v>0.99272600934203192</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>65</v>
       </c>
       <c r="B47">
         <v>0.99188942959358262</v>
       </c>
-      <c r="E47" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>66</v>
       </c>

</xml_diff>